<commit_message>
add new row data & Insert empty rows
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1,57 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tariq\projectsWSL\python\working with sheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price </t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[Red]\-[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -351,68 +386,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col width="11.5703125" customWidth="1" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>transaction_id</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">price </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="1" t="n">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="n">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="n">
+        <v>6.95</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2">
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>5.95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3">
+      <c r="B6" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4">
+      <c r="C6" t="n">
         <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7.95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moving a range of cells
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -391,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -402,65 +402,54 @@
     <col width="11.5703125" customWidth="1" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>transaction_id</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>product_id</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t xml:space="preserve">price </t>
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>5.95</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>5.95</v>
+        <v>6.95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>6.95</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="n">
         <v>7.95</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>